<commit_message>
Added institutionCode, collectionCode, and catalogNumber to make triple
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="156">
   <si>
     <t>Taxon</t>
   </si>
@@ -472,6 +472,21 @@
   </si>
   <si>
     <t>LITERATURE</t>
+  </si>
+  <si>
+    <t>collectionCode</t>
+  </si>
+  <si>
+    <t>institutionCode</t>
+  </si>
+  <si>
+    <t>catalogNumber</t>
+  </si>
+  <si>
+    <t>10.1016/j.ympev.2006.04.006</t>
+  </si>
+  <si>
+    <t>IBACM</t>
   </si>
 </sst>
 </file>
@@ -528,8 +543,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -549,7 +570,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -557,6 +578,9 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -564,6 +588,9 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -893,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI22"/>
+  <dimension ref="A1:AL22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AA28" sqref="AA28"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:AL22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -905,16 +932,19 @@
     <col min="11" max="12" width="18.5" customWidth="1"/>
     <col min="17" max="17" width="13.5" customWidth="1"/>
     <col min="24" max="24" width="36.6640625" customWidth="1"/>
-    <col min="25" max="25" width="22.33203125" customWidth="1"/>
-    <col min="26" max="27" width="35" customWidth="1"/>
-    <col min="30" max="30" width="13.6640625" customWidth="1"/>
-    <col min="31" max="31" width="13.83203125" customWidth="1"/>
-    <col min="32" max="32" width="18.33203125" customWidth="1"/>
-    <col min="33" max="33" width="17.6640625" customWidth="1"/>
-    <col min="34" max="34" width="24.1640625" customWidth="1"/>
+    <col min="25" max="25" width="17" customWidth="1"/>
+    <col min="26" max="26" width="27.83203125" customWidth="1"/>
+    <col min="27" max="27" width="15.33203125" customWidth="1"/>
+    <col min="28" max="28" width="22.33203125" customWidth="1"/>
+    <col min="29" max="30" width="35" customWidth="1"/>
+    <col min="33" max="33" width="13.6640625" customWidth="1"/>
+    <col min="34" max="34" width="13.83203125" customWidth="1"/>
+    <col min="35" max="35" width="18.33203125" customWidth="1"/>
+    <col min="36" max="36" width="17.6640625" customWidth="1"/>
+    <col min="37" max="37" width="24.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:38">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -979,40 +1009,49 @@
         <v>133</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:38">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1095,50 +1134,60 @@
       <c r="X2" t="s">
         <v>135</v>
       </c>
-      <c r="Y2" t="str">
+      <c r="Y2" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA2">
+        <f>W2</f>
+        <v>1</v>
+      </c>
+      <c r="AB2" t="str">
         <f>K2</f>
         <v>Banza nihoa</v>
       </c>
-      <c r="Z2" t="str">
+      <c r="AC2" t="str">
         <f>IF(L2&lt;&gt;"",CONCATENATE("http://www.gbif.org/species/",L2),"")</f>
         <v>http://www.gbif.org/species/1689137</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AD2" t="s">
         <v>150</v>
       </c>
-      <c r="AB2" t="str">
+      <c r="AE2" t="str">
         <f>B2</f>
         <v>Nihoa</v>
       </c>
-      <c r="AC2" t="str">
+      <c r="AF2" t="str">
         <f>C2</f>
         <v>Miller Peak</v>
       </c>
-      <c r="AD2" t="str">
+      <c r="AG2" t="str">
         <f>D2</f>
         <v>23°03′44′′N</v>
       </c>
-      <c r="AE2" t="str">
+      <c r="AH2" t="str">
         <f>E2</f>
         <v>161°55′34′′W</v>
       </c>
-      <c r="AF2">
+      <c r="AI2">
         <f>Q2</f>
         <v>23.062222222222221</v>
       </c>
-      <c r="AG2">
+      <c r="AJ2">
         <f>V2</f>
         <v>-161.92611111111111</v>
       </c>
-      <c r="AH2" t="str">
+      <c r="AK2" t="str">
         <f>CONCATENATE(F2,"|",G2)</f>
         <v>DQ649491|DQ649515</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AL2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:38">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1221,50 +1270,60 @@
       <c r="X3" t="s">
         <v>135</v>
       </c>
-      <c r="Y3" t="str">
-        <f t="shared" ref="Y3:Y22" si="13">K3</f>
+      <c r="Y3" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA3">
+        <f t="shared" ref="AA3:AA22" si="13">W3</f>
+        <v>2</v>
+      </c>
+      <c r="AB3" t="str">
+        <f t="shared" ref="AB3:AB22" si="14">K3</f>
         <v>Banza nihoa</v>
       </c>
-      <c r="Z3" t="str">
-        <f t="shared" ref="Z3:Z22" si="14">IF(L3&lt;&gt;"",CONCATENATE("http://www.gbif.org/species/",L3),"")</f>
+      <c r="AC3" t="str">
+        <f t="shared" ref="AC3:AC22" si="15">IF(L3&lt;&gt;"",CONCATENATE("http://www.gbif.org/species/",L3),"")</f>
         <v>http://www.gbif.org/species/1689137</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AD3" t="s">
         <v>150</v>
       </c>
-      <c r="AB3" t="str">
-        <f t="shared" ref="AB3:AB22" si="15">B3</f>
+      <c r="AE3" t="str">
+        <f t="shared" ref="AE3:AE22" si="16">B3</f>
         <v>Nihoa</v>
       </c>
-      <c r="AC3" t="str">
-        <f t="shared" ref="AC3:AC22" si="16">C3</f>
+      <c r="AF3" t="str">
+        <f t="shared" ref="AF3:AF22" si="17">C3</f>
         <v>Miller Peak</v>
       </c>
-      <c r="AD3" t="str">
-        <f t="shared" ref="AD3:AD22" si="17">D3</f>
+      <c r="AG3" t="str">
+        <f t="shared" ref="AG3:AG22" si="18">D3</f>
         <v>23°03′44′′N</v>
       </c>
-      <c r="AE3" t="str">
-        <f t="shared" ref="AE3:AE22" si="18">E3</f>
+      <c r="AH3" t="str">
+        <f t="shared" ref="AH3:AH22" si="19">E3</f>
         <v>161°55′34′′W</v>
       </c>
-      <c r="AF3">
-        <f t="shared" ref="AF3:AF22" si="19">Q3</f>
+      <c r="AI3">
+        <f t="shared" ref="AI3:AI22" si="20">Q3</f>
         <v>23.062222222222221</v>
       </c>
-      <c r="AG3">
-        <f t="shared" ref="AG3:AG22" si="20">V3</f>
+      <c r="AJ3">
+        <f t="shared" ref="AJ3:AJ22" si="21">V3</f>
         <v>-161.92611111111111</v>
       </c>
-      <c r="AH3" t="str">
-        <f t="shared" ref="AH3:AH21" si="21">CONCATENATE(F3,"|",G3)</f>
+      <c r="AK3" t="str">
+        <f t="shared" ref="AK3:AK21" si="22">CONCATENATE(F3,"|",G3)</f>
         <v>DQ649492|DQ649516</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AL3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:38">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1347,50 +1406,60 @@
       <c r="X4" t="s">
         <v>135</v>
       </c>
-      <c r="Y4" t="str">
+      <c r="Y4" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA4">
         <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="AB4" t="str">
+        <f t="shared" si="14"/>
         <v>Banza kauaiensis</v>
       </c>
-      <c r="Z4" t="str">
-        <f t="shared" si="14"/>
+      <c r="AC4" t="str">
+        <f t="shared" si="15"/>
         <v>http://www.gbif.org/species/1689120</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AD4" t="s">
         <v>150</v>
       </c>
-      <c r="AB4" t="str">
-        <f t="shared" si="15"/>
+      <c r="AE4" t="str">
+        <f t="shared" si="16"/>
         <v>Kauai</v>
       </c>
-      <c r="AC4" t="str">
-        <f t="shared" si="16"/>
+      <c r="AF4" t="str">
+        <f t="shared" si="17"/>
         <v>Alexander Dam</v>
       </c>
-      <c r="AD4" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG4" t="str">
+        <f t="shared" si="18"/>
         <v>21°58′30′′N</v>
       </c>
-      <c r="AE4" t="str">
-        <f t="shared" si="18"/>
+      <c r="AH4" t="str">
+        <f t="shared" si="19"/>
         <v>159°27′58′′W</v>
       </c>
-      <c r="AF4">
-        <f t="shared" si="19"/>
+      <c r="AI4">
+        <f t="shared" si="20"/>
         <v>21.974999999999998</v>
       </c>
-      <c r="AG4">
-        <f t="shared" si="20"/>
+      <c r="AJ4">
+        <f t="shared" si="21"/>
         <v>-159.4661111111111</v>
       </c>
-      <c r="AH4" t="str">
-        <f t="shared" si="21"/>
+      <c r="AK4" t="str">
+        <f t="shared" si="22"/>
         <v>DQ649483|DQ649507</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AL4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:38">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1473,50 +1542,60 @@
       <c r="X5" t="s">
         <v>135</v>
       </c>
-      <c r="Y5" t="str">
+      <c r="Y5" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA5">
         <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="AB5" t="str">
+        <f t="shared" si="14"/>
         <v>Banza kauaiensis</v>
       </c>
-      <c r="Z5" t="str">
-        <f t="shared" si="14"/>
+      <c r="AC5" t="str">
+        <f t="shared" si="15"/>
         <v>http://www.gbif.org/species/1689120</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AD5" t="s">
         <v>150</v>
       </c>
-      <c r="AB5" t="str">
-        <f t="shared" si="15"/>
+      <c r="AE5" t="str">
+        <f t="shared" si="16"/>
         <v>Kauai</v>
       </c>
-      <c r="AC5" t="str">
-        <f t="shared" si="16"/>
+      <c r="AF5" t="str">
+        <f t="shared" si="17"/>
         <v>Kokee, Pihea Trail</v>
       </c>
-      <c r="AD5" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG5" t="str">
+        <f t="shared" si="18"/>
         <v>22°09′14′′N</v>
       </c>
-      <c r="AE5" t="str">
-        <f t="shared" si="18"/>
+      <c r="AH5" t="str">
+        <f t="shared" si="19"/>
         <v>159°37′30′′W</v>
       </c>
-      <c r="AF5">
-        <f t="shared" si="19"/>
+      <c r="AI5">
+        <f t="shared" si="20"/>
         <v>22.153888888888886</v>
       </c>
-      <c r="AG5">
-        <f t="shared" si="20"/>
+      <c r="AJ5">
+        <f t="shared" si="21"/>
         <v>-159.625</v>
       </c>
-      <c r="AH5" t="str">
-        <f t="shared" si="21"/>
+      <c r="AK5" t="str">
+        <f t="shared" si="22"/>
         <v>DQ649484|DQ649508</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AL5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:38">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1599,50 +1678,60 @@
       <c r="X6" t="s">
         <v>135</v>
       </c>
-      <c r="Y6" t="str">
+      <c r="Y6" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA6">
         <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="AB6" t="str">
+        <f t="shared" si="14"/>
         <v>Banza unica</v>
       </c>
-      <c r="Z6" t="str">
-        <f t="shared" si="14"/>
+      <c r="AC6" t="str">
+        <f t="shared" si="15"/>
         <v>http://www.gbif.org/species/1689133</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AD6" t="s">
         <v>150</v>
       </c>
-      <c r="AB6" t="str">
-        <f t="shared" si="15"/>
+      <c r="AE6" t="str">
+        <f t="shared" si="16"/>
         <v>Oahu</v>
       </c>
-      <c r="AC6" t="str">
-        <f t="shared" si="16"/>
+      <c r="AF6" t="str">
+        <f t="shared" si="17"/>
         <v>Mount Tantalus</v>
       </c>
-      <c r="AD6" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG6" t="str">
+        <f t="shared" si="18"/>
         <v>21°20′14′′N</v>
       </c>
-      <c r="AE6" t="str">
-        <f t="shared" si="18"/>
+      <c r="AH6" t="str">
+        <f t="shared" si="19"/>
         <v>157°49′04′′W</v>
       </c>
-      <c r="AF6">
-        <f t="shared" si="19"/>
+      <c r="AI6">
+        <f t="shared" si="20"/>
         <v>21.33722222222222</v>
       </c>
-      <c r="AG6">
-        <f t="shared" si="20"/>
+      <c r="AJ6">
+        <f t="shared" si="21"/>
         <v>-157.81777777777776</v>
       </c>
-      <c r="AH6" t="str">
-        <f t="shared" si="21"/>
+      <c r="AK6" t="str">
+        <f t="shared" si="22"/>
         <v>DQ649501|DQ649525</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AL6" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:38">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1725,50 +1814,60 @@
       <c r="X7" t="s">
         <v>135</v>
       </c>
-      <c r="Y7" t="str">
+      <c r="Y7" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA7">
         <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="AB7" t="str">
+        <f t="shared" si="14"/>
         <v>Banza unica</v>
       </c>
-      <c r="Z7" t="str">
-        <f t="shared" si="14"/>
+      <c r="AC7" t="str">
+        <f t="shared" si="15"/>
         <v>http://www.gbif.org/species/1689133</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AD7" t="s">
         <v>150</v>
       </c>
-      <c r="AB7" t="str">
-        <f t="shared" si="15"/>
+      <c r="AE7" t="str">
+        <f t="shared" si="16"/>
         <v>Oahu</v>
       </c>
-      <c r="AC7" t="str">
-        <f t="shared" si="16"/>
+      <c r="AF7" t="str">
+        <f t="shared" si="17"/>
         <v>Palikea Trail</v>
       </c>
-      <c r="AD7" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG7" t="str">
+        <f t="shared" si="18"/>
         <v>21°24′59′′N</v>
       </c>
-      <c r="AE7" t="str">
-        <f t="shared" si="18"/>
+      <c r="AH7" t="str">
+        <f t="shared" si="19"/>
         <v>158°06′13′′W</v>
       </c>
-      <c r="AF7">
-        <f t="shared" si="19"/>
+      <c r="AI7">
+        <f t="shared" si="20"/>
         <v>21.416388888888889</v>
       </c>
-      <c r="AG7">
-        <f t="shared" si="20"/>
+      <c r="AJ7">
+        <f t="shared" si="21"/>
         <v>-158.10361111111109</v>
       </c>
-      <c r="AH7" t="str">
-        <f t="shared" si="21"/>
+      <c r="AK7" t="str">
+        <f t="shared" si="22"/>
         <v>DQ649502|DQ649526</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AL7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:38">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1851,50 +1950,60 @@
       <c r="X8" t="s">
         <v>135</v>
       </c>
-      <c r="Y8" t="str">
+      <c r="Y8" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA8">
         <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="AB8" t="str">
+        <f t="shared" si="14"/>
         <v>Banza parvula</v>
       </c>
-      <c r="Z8" t="str">
-        <f t="shared" si="14"/>
+      <c r="AC8" t="str">
+        <f t="shared" si="15"/>
         <v>http://www.gbif.org/species/1689127</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AD8" t="s">
         <v>150</v>
       </c>
-      <c r="AB8" t="str">
-        <f t="shared" si="15"/>
+      <c r="AE8" t="str">
+        <f t="shared" si="16"/>
         <v>Oahu</v>
       </c>
-      <c r="AC8" t="str">
-        <f t="shared" si="16"/>
+      <c r="AF8" t="str">
+        <f t="shared" si="17"/>
         <v>Puu Kaua</v>
       </c>
-      <c r="AD8" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG8" t="str">
+        <f t="shared" si="18"/>
         <v>21°26′41′′N</v>
       </c>
-      <c r="AE8" t="str">
-        <f t="shared" si="18"/>
+      <c r="AH8" t="str">
+        <f t="shared" si="19"/>
         <v>158°06′05′′W</v>
       </c>
-      <c r="AF8">
-        <f t="shared" si="19"/>
+      <c r="AI8">
+        <f t="shared" si="20"/>
         <v>21.444722222222222</v>
       </c>
-      <c r="AG8">
-        <f t="shared" si="20"/>
+      <c r="AJ8">
+        <f t="shared" si="21"/>
         <v>-158.10138888888889</v>
       </c>
-      <c r="AH8" t="str">
-        <f t="shared" si="21"/>
+      <c r="AK8" t="str">
+        <f t="shared" si="22"/>
         <v>DQ649497|DQ649521</v>
       </c>
-      <c r="AI8" t="s">
+      <c r="AL8" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:38">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -1977,50 +2086,60 @@
       <c r="X9" t="s">
         <v>135</v>
       </c>
-      <c r="Y9" t="str">
+      <c r="Y9" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA9">
         <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="AB9" t="str">
+        <f t="shared" si="14"/>
         <v>Banza parvula</v>
       </c>
-      <c r="Z9" t="str">
-        <f t="shared" si="14"/>
+      <c r="AC9" t="str">
+        <f t="shared" si="15"/>
         <v>http://www.gbif.org/species/1689127</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AD9" t="s">
         <v>150</v>
       </c>
-      <c r="AB9" t="str">
-        <f t="shared" si="15"/>
+      <c r="AE9" t="str">
+        <f t="shared" si="16"/>
         <v>Oahu</v>
       </c>
-      <c r="AC9" t="str">
-        <f t="shared" si="16"/>
+      <c r="AF9" t="str">
+        <f t="shared" si="17"/>
         <v>Peacock Flats</v>
       </c>
-      <c r="AD9" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG9" t="str">
+        <f t="shared" si="18"/>
         <v>21°32′57′′N</v>
       </c>
-      <c r="AE9" t="str">
-        <f t="shared" si="18"/>
+      <c r="AH9" t="str">
+        <f t="shared" si="19"/>
         <v>158°11′13′′W</v>
       </c>
-      <c r="AF9">
-        <f t="shared" si="19"/>
+      <c r="AI9">
+        <f t="shared" si="20"/>
         <v>21.549166666666668</v>
       </c>
-      <c r="AG9">
-        <f t="shared" si="20"/>
+      <c r="AJ9">
+        <f t="shared" si="21"/>
         <v>-158.18694444444444</v>
       </c>
-      <c r="AH9" t="str">
-        <f t="shared" si="21"/>
+      <c r="AK9" t="str">
+        <f t="shared" si="22"/>
         <v>DQ649498|DQ649522</v>
       </c>
-      <c r="AI9" t="s">
+      <c r="AL9" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:38">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -2103,50 +2222,60 @@
       <c r="X10" t="s">
         <v>135</v>
       </c>
-      <c r="Y10" t="str">
+      <c r="Y10" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA10">
         <f t="shared" si="13"/>
+        <v>9</v>
+      </c>
+      <c r="AB10" t="str">
+        <f t="shared" si="14"/>
         <v>Banza molokaiensis</v>
       </c>
-      <c r="Z10" t="str">
-        <f t="shared" si="14"/>
+      <c r="AC10" t="str">
+        <f t="shared" si="15"/>
         <v>http://www.gbif.org/species/1689135</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AD10" t="s">
         <v>150</v>
       </c>
-      <c r="AB10" t="str">
-        <f t="shared" si="15"/>
+      <c r="AE10" t="str">
+        <f t="shared" si="16"/>
         <v>Molokai</v>
       </c>
-      <c r="AC10" t="str">
-        <f t="shared" si="16"/>
+      <c r="AF10" t="str">
+        <f t="shared" si="17"/>
         <v>Puu Kole Kole</v>
       </c>
-      <c r="AD10" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG10" t="str">
+        <f t="shared" si="18"/>
         <v>21°06′35′′N</v>
       </c>
-      <c r="AE10" t="str">
-        <f t="shared" si="18"/>
+      <c r="AH10" t="str">
+        <f t="shared" si="19"/>
         <v>156°54′10′′W</v>
       </c>
-      <c r="AF10">
-        <f t="shared" si="19"/>
+      <c r="AI10">
+        <f t="shared" si="20"/>
         <v>21.109722222222224</v>
       </c>
-      <c r="AG10">
-        <f t="shared" si="20"/>
+      <c r="AJ10">
+        <f t="shared" si="21"/>
         <v>-156.90277777777777</v>
       </c>
-      <c r="AH10" t="str">
-        <f t="shared" si="21"/>
+      <c r="AK10" t="str">
+        <f t="shared" si="22"/>
         <v>DQ649487|DQ649511</v>
       </c>
-      <c r="AI10" t="s">
+      <c r="AL10" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:38">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -2229,50 +2358,60 @@
       <c r="X11" t="s">
         <v>135</v>
       </c>
-      <c r="Y11" t="str">
+      <c r="Y11" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA11">
         <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="AB11" t="str">
+        <f t="shared" si="14"/>
         <v>Banza molokaiensis</v>
       </c>
-      <c r="Z11" t="str">
-        <f t="shared" si="14"/>
+      <c r="AC11" t="str">
+        <f t="shared" si="15"/>
         <v>http://www.gbif.org/species/1689135</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AD11" t="s">
         <v>150</v>
       </c>
-      <c r="AB11" t="str">
-        <f t="shared" si="15"/>
+      <c r="AE11" t="str">
+        <f t="shared" si="16"/>
         <v>Molokai</v>
       </c>
-      <c r="AC11" t="str">
-        <f t="shared" si="16"/>
+      <c r="AF11" t="str">
+        <f t="shared" si="17"/>
         <v>Puu Kole Kole</v>
       </c>
-      <c r="AD11" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG11" t="str">
+        <f t="shared" si="18"/>
         <v>21°06′35′′N</v>
       </c>
-      <c r="AE11" t="str">
-        <f t="shared" si="18"/>
+      <c r="AH11" t="str">
+        <f t="shared" si="19"/>
         <v>156°54′10′′W</v>
       </c>
-      <c r="AF11">
-        <f t="shared" si="19"/>
+      <c r="AI11">
+        <f t="shared" si="20"/>
         <v>21.109722222222224</v>
       </c>
-      <c r="AG11">
-        <f t="shared" si="20"/>
+      <c r="AJ11">
+        <f t="shared" si="21"/>
         <v>-156.90277777777777</v>
       </c>
-      <c r="AH11" t="str">
-        <f t="shared" si="21"/>
+      <c r="AK11" t="str">
+        <f t="shared" si="22"/>
         <v>DQ649488|DQ649512</v>
       </c>
-      <c r="AI11" t="s">
+      <c r="AL11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:38">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -2355,50 +2494,60 @@
       <c r="X12" t="s">
         <v>135</v>
       </c>
-      <c r="Y12" t="str">
+      <c r="Y12" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA12">
         <f t="shared" si="13"/>
+        <v>11</v>
+      </c>
+      <c r="AB12" t="str">
+        <f t="shared" si="14"/>
         <v>Banza deplanata</v>
       </c>
-      <c r="Z12" t="str">
-        <f t="shared" si="14"/>
+      <c r="AC12" t="str">
+        <f t="shared" si="15"/>
         <v>http://www.gbif.org/species/1689124</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AD12" t="s">
         <v>150</v>
       </c>
-      <c r="AB12" t="str">
-        <f t="shared" si="15"/>
+      <c r="AE12" t="str">
+        <f t="shared" si="16"/>
         <v>Lanai</v>
       </c>
-      <c r="AC12" t="str">
-        <f t="shared" si="16"/>
+      <c r="AF12" t="str">
+        <f t="shared" si="17"/>
         <v>Lanaihale</v>
       </c>
-      <c r="AD12" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG12" t="str">
+        <f t="shared" si="18"/>
         <v>20°48′53′′N</v>
       </c>
-      <c r="AE12" t="str">
-        <f t="shared" si="18"/>
+      <c r="AH12" t="str">
+        <f t="shared" si="19"/>
         <v>156°52′33′′W</v>
       </c>
-      <c r="AF12">
-        <f t="shared" si="19"/>
+      <c r="AI12">
+        <f t="shared" si="20"/>
         <v>20.814722222222223</v>
       </c>
-      <c r="AG12">
-        <f t="shared" si="20"/>
+      <c r="AJ12">
+        <f t="shared" si="21"/>
         <v>-156.87583333333333</v>
       </c>
-      <c r="AH12" t="str">
-        <f t="shared" si="21"/>
+      <c r="AK12" t="str">
+        <f t="shared" si="22"/>
         <v>DQ649481|DQ649505</v>
       </c>
-      <c r="AI12" t="s">
+      <c r="AL12" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:38">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -2481,50 +2630,60 @@
       <c r="X13" t="s">
         <v>135</v>
       </c>
-      <c r="Y13" t="str">
+      <c r="Y13" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA13">
         <f t="shared" si="13"/>
+        <v>12</v>
+      </c>
+      <c r="AB13" t="str">
+        <f t="shared" si="14"/>
         <v>Banza deplanata</v>
       </c>
-      <c r="Z13" t="str">
-        <f t="shared" si="14"/>
+      <c r="AC13" t="str">
+        <f t="shared" si="15"/>
         <v>http://www.gbif.org/species/1689124</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AD13" t="s">
         <v>150</v>
       </c>
-      <c r="AB13" t="str">
-        <f t="shared" si="15"/>
+      <c r="AE13" t="str">
+        <f t="shared" si="16"/>
         <v>Lanai</v>
       </c>
-      <c r="AC13" t="str">
-        <f t="shared" si="16"/>
+      <c r="AF13" t="str">
+        <f t="shared" si="17"/>
         <v>Lanaihale</v>
       </c>
-      <c r="AD13" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG13" t="str">
+        <f t="shared" si="18"/>
         <v>20°48′53′′N</v>
       </c>
-      <c r="AE13" t="str">
-        <f t="shared" si="18"/>
+      <c r="AH13" t="str">
+        <f t="shared" si="19"/>
         <v>156°52′14′′W</v>
       </c>
-      <c r="AF13">
-        <f t="shared" si="19"/>
+      <c r="AI13">
+        <f t="shared" si="20"/>
         <v>20.814722222222223</v>
       </c>
-      <c r="AG13">
-        <f t="shared" si="20"/>
+      <c r="AJ13">
+        <f t="shared" si="21"/>
         <v>-156.87055555555557</v>
       </c>
-      <c r="AH13" t="str">
-        <f t="shared" si="21"/>
+      <c r="AK13" t="str">
+        <f t="shared" si="22"/>
         <v>DQ649482|DQ649506</v>
       </c>
-      <c r="AI13" t="s">
+      <c r="AL13" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:38">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -2607,50 +2766,60 @@
       <c r="X14" t="s">
         <v>135</v>
       </c>
-      <c r="Y14" t="str">
+      <c r="Y14" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA14">
         <f t="shared" si="13"/>
+        <v>13</v>
+      </c>
+      <c r="AB14" t="str">
+        <f t="shared" si="14"/>
         <v>Banza brunnea</v>
       </c>
-      <c r="Z14" t="str">
-        <f t="shared" si="14"/>
+      <c r="AC14" t="str">
+        <f t="shared" si="15"/>
         <v>http://www.gbif.org/species/1689144</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AD14" t="s">
         <v>150</v>
       </c>
-      <c r="AB14" t="str">
-        <f t="shared" si="15"/>
+      <c r="AE14" t="str">
+        <f t="shared" si="16"/>
         <v>Maui (West)</v>
       </c>
-      <c r="AC14" t="str">
-        <f t="shared" si="16"/>
+      <c r="AF14" t="str">
+        <f t="shared" si="17"/>
         <v>Kaulalewelewe</v>
       </c>
-      <c r="AD14" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG14" t="str">
+        <f t="shared" si="18"/>
         <v>20°56′14′′N</v>
       </c>
-      <c r="AE14" t="str">
-        <f t="shared" si="18"/>
+      <c r="AH14" t="str">
+        <f t="shared" si="19"/>
         <v>156°37′10′′W</v>
       </c>
-      <c r="AF14">
-        <f t="shared" si="19"/>
+      <c r="AI14">
+        <f t="shared" si="20"/>
         <v>20.937222222222221</v>
       </c>
-      <c r="AG14">
-        <f t="shared" si="20"/>
+      <c r="AJ14">
+        <f t="shared" si="21"/>
         <v>-156.61944444444444</v>
       </c>
-      <c r="AH14" t="str">
-        <f t="shared" si="21"/>
+      <c r="AK14" t="str">
+        <f t="shared" si="22"/>
         <v>DQ649479|DQ649503</v>
       </c>
-      <c r="AI14" t="s">
+      <c r="AL14" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:38">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -2733,50 +2902,60 @@
       <c r="X15" t="s">
         <v>135</v>
       </c>
-      <c r="Y15" t="str">
+      <c r="Y15" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA15">
         <f t="shared" si="13"/>
+        <v>14</v>
+      </c>
+      <c r="AB15" t="str">
+        <f t="shared" si="14"/>
         <v>Banza brunnea</v>
       </c>
-      <c r="Z15" t="str">
-        <f t="shared" si="14"/>
+      <c r="AC15" t="str">
+        <f t="shared" si="15"/>
         <v>http://www.gbif.org/species/1689144</v>
       </c>
-      <c r="AA15" t="s">
+      <c r="AD15" t="s">
         <v>150</v>
       </c>
-      <c r="AB15" t="str">
-        <f t="shared" si="15"/>
+      <c r="AE15" t="str">
+        <f t="shared" si="16"/>
         <v>Maui (West)</v>
       </c>
-      <c r="AC15" t="str">
-        <f t="shared" si="16"/>
+      <c r="AF15" t="str">
+        <f t="shared" si="17"/>
         <v>Lihau</v>
       </c>
-      <c r="AD15" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG15" t="str">
+        <f t="shared" si="18"/>
         <v>20°51′18′′N</v>
       </c>
-      <c r="AE15" t="str">
-        <f t="shared" si="18"/>
+      <c r="AH15" t="str">
+        <f t="shared" si="19"/>
         <v>156°36′12′′W</v>
       </c>
-      <c r="AF15">
-        <f t="shared" si="19"/>
+      <c r="AI15">
+        <f t="shared" si="20"/>
         <v>20.855</v>
       </c>
-      <c r="AG15">
-        <f t="shared" si="20"/>
+      <c r="AJ15">
+        <f t="shared" si="21"/>
         <v>-156.60333333333332</v>
       </c>
-      <c r="AH15" t="str">
-        <f t="shared" si="21"/>
+      <c r="AK15" t="str">
+        <f t="shared" si="22"/>
         <v>DQ649480|DQ649504</v>
       </c>
-      <c r="AI15" t="s">
+      <c r="AL15" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:38">
       <c r="A16" t="s">
         <v>89</v>
       </c>
@@ -2859,50 +3038,60 @@
       <c r="X16" t="s">
         <v>135</v>
       </c>
-      <c r="Y16" t="str">
+      <c r="Y16" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA16">
         <f t="shared" si="13"/>
+        <v>15</v>
+      </c>
+      <c r="AB16" t="str">
+        <f t="shared" si="14"/>
         <v>Banza mauiensis</v>
       </c>
-      <c r="Z16" t="str">
-        <f t="shared" si="14"/>
+      <c r="AC16" t="str">
+        <f t="shared" si="15"/>
         <v>http://www.gbif.org/species/1689122</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="AD16" t="s">
         <v>150</v>
       </c>
-      <c r="AB16" t="str">
-        <f t="shared" si="15"/>
+      <c r="AE16" t="str">
+        <f t="shared" si="16"/>
         <v>Maui (West)</v>
       </c>
-      <c r="AC16" t="str">
-        <f t="shared" si="16"/>
+      <c r="AF16" t="str">
+        <f t="shared" si="17"/>
         <v>Hanaula</v>
       </c>
-      <c r="AD16" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG16" t="str">
+        <f t="shared" si="18"/>
         <v>20°50′42′′N</v>
       </c>
-      <c r="AE16" t="str">
-        <f t="shared" si="18"/>
+      <c r="AH16" t="str">
+        <f t="shared" si="19"/>
         <v>156°33′26′′W</v>
       </c>
-      <c r="AF16">
-        <f t="shared" si="19"/>
+      <c r="AI16">
+        <f t="shared" si="20"/>
         <v>20.844999999999999</v>
       </c>
-      <c r="AG16">
-        <f t="shared" si="20"/>
+      <c r="AJ16">
+        <f t="shared" si="21"/>
         <v>-156.55722222222224</v>
       </c>
-      <c r="AH16" t="str">
-        <f t="shared" si="21"/>
+      <c r="AK16" t="str">
+        <f t="shared" si="22"/>
         <v>DQ649485|DQ649509</v>
       </c>
-      <c r="AI16" t="s">
+      <c r="AL16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:38">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -2985,50 +3174,60 @@
       <c r="X17" t="s">
         <v>135</v>
       </c>
-      <c r="Y17" t="str">
+      <c r="Y17" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA17">
         <f t="shared" si="13"/>
+        <v>16</v>
+      </c>
+      <c r="AB17" t="str">
+        <f t="shared" si="14"/>
         <v>Banza mauiensis</v>
       </c>
-      <c r="Z17" t="str">
-        <f t="shared" si="14"/>
+      <c r="AC17" t="str">
+        <f t="shared" si="15"/>
         <v>http://www.gbif.org/species/1689122</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="AD17" t="s">
         <v>150</v>
       </c>
-      <c r="AB17" t="str">
-        <f t="shared" si="15"/>
+      <c r="AE17" t="str">
+        <f t="shared" si="16"/>
         <v>Maui (West)</v>
       </c>
-      <c r="AC17" t="str">
-        <f t="shared" si="16"/>
+      <c r="AF17" t="str">
+        <f t="shared" si="17"/>
         <v>Hanaula</v>
       </c>
-      <c r="AD17" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG17" t="str">
+        <f t="shared" si="18"/>
         <v>20°50′42′′N</v>
       </c>
-      <c r="AE17" t="str">
-        <f t="shared" si="18"/>
+      <c r="AH17" t="str">
+        <f t="shared" si="19"/>
         <v>156°33′26′′W</v>
       </c>
-      <c r="AF17">
-        <f t="shared" si="19"/>
+      <c r="AI17">
+        <f t="shared" si="20"/>
         <v>20.844999999999999</v>
       </c>
-      <c r="AG17">
-        <f t="shared" si="20"/>
+      <c r="AJ17">
+        <f t="shared" si="21"/>
         <v>-156.55722222222224</v>
       </c>
-      <c r="AH17" t="str">
-        <f t="shared" si="21"/>
+      <c r="AK17" t="str">
+        <f t="shared" si="22"/>
         <v>DQ649486|DQ649510</v>
       </c>
-      <c r="AI17" t="s">
+      <c r="AL17" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:38">
       <c r="A18" t="s">
         <v>145</v>
       </c>
@@ -3108,50 +3307,60 @@
       <c r="X18" t="s">
         <v>135</v>
       </c>
-      <c r="Y18" t="str">
+      <c r="Y18" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA18">
         <f t="shared" si="13"/>
+        <v>17</v>
+      </c>
+      <c r="AB18" t="str">
+        <f t="shared" si="14"/>
         <v>Banza "pilimauiensis"</v>
       </c>
-      <c r="Z18" t="str">
-        <f t="shared" si="14"/>
+      <c r="AC18" t="str">
+        <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AA18" t="s">
+      <c r="AD18" t="s">
         <v>150</v>
       </c>
-      <c r="AB18" t="str">
-        <f t="shared" si="15"/>
+      <c r="AE18" t="str">
+        <f t="shared" si="16"/>
         <v>Maui (East)</v>
       </c>
-      <c r="AC18" t="str">
-        <f t="shared" si="16"/>
+      <c r="AF18" t="str">
+        <f t="shared" si="17"/>
         <v>Waikamoi</v>
       </c>
-      <c r="AD18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG18" t="str">
+        <f t="shared" si="18"/>
         <v>20°49′04′′N</v>
       </c>
-      <c r="AE18" t="str">
-        <f t="shared" si="18"/>
+      <c r="AH18" t="str">
+        <f t="shared" si="19"/>
         <v>156°13′49′′W</v>
       </c>
-      <c r="AF18">
-        <f t="shared" si="19"/>
+      <c r="AI18">
+        <f t="shared" si="20"/>
         <v>20.817777777777778</v>
       </c>
-      <c r="AG18">
-        <f t="shared" si="20"/>
+      <c r="AJ18">
+        <f t="shared" si="21"/>
         <v>-156.23027777777779</v>
       </c>
-      <c r="AH18" t="str">
-        <f t="shared" si="21"/>
+      <c r="AK18" t="str">
+        <f t="shared" si="22"/>
         <v>DQ649499|DQ649523</v>
       </c>
-      <c r="AI18" t="s">
+      <c r="AL18" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:38">
       <c r="A19" t="s">
         <v>146</v>
       </c>
@@ -3231,50 +3440,60 @@
       <c r="X19" t="s">
         <v>135</v>
       </c>
-      <c r="Y19" t="str">
+      <c r="Y19" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA19">
         <f t="shared" si="13"/>
+        <v>18</v>
+      </c>
+      <c r="AB19" t="str">
+        <f t="shared" si="14"/>
         <v>Banza "pilimauiensis"</v>
       </c>
-      <c r="Z19" t="str">
-        <f t="shared" si="14"/>
+      <c r="AC19" t="str">
+        <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AA19" t="s">
+      <c r="AD19" t="s">
         <v>150</v>
       </c>
-      <c r="AB19" t="str">
-        <f t="shared" si="15"/>
+      <c r="AE19" t="str">
+        <f t="shared" si="16"/>
         <v>Maui (East)</v>
       </c>
-      <c r="AC19" t="str">
-        <f t="shared" si="16"/>
+      <c r="AF19" t="str">
+        <f t="shared" si="17"/>
         <v>Waikamoi</v>
       </c>
-      <c r="AD19" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG19" t="str">
+        <f t="shared" si="18"/>
         <v>20°49′04′′N</v>
       </c>
-      <c r="AE19" t="str">
-        <f t="shared" si="18"/>
+      <c r="AH19" t="str">
+        <f t="shared" si="19"/>
         <v>156°13′49′′W</v>
       </c>
-      <c r="AF19">
-        <f t="shared" si="19"/>
+      <c r="AI19">
+        <f t="shared" si="20"/>
         <v>20.817777777777778</v>
       </c>
-      <c r="AG19">
-        <f t="shared" si="20"/>
+      <c r="AJ19">
+        <f t="shared" si="21"/>
         <v>-156.23027777777779</v>
       </c>
-      <c r="AH19" t="str">
-        <f t="shared" si="21"/>
+      <c r="AK19" t="str">
+        <f t="shared" si="22"/>
         <v>DQ649500|DQ649524</v>
       </c>
-      <c r="AI19" t="s">
+      <c r="AL19" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:38">
       <c r="A20" t="s">
         <v>106</v>
       </c>
@@ -3357,50 +3576,60 @@
       <c r="X20" t="s">
         <v>135</v>
       </c>
-      <c r="Y20" t="str">
+      <c r="Y20" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA20">
         <f t="shared" si="13"/>
+        <v>19</v>
+      </c>
+      <c r="AB20" t="str">
+        <f t="shared" si="14"/>
         <v>Banza nitida</v>
       </c>
-      <c r="Z20" t="str">
-        <f t="shared" si="14"/>
+      <c r="AC20" t="str">
+        <f t="shared" si="15"/>
         <v>http://www.gbif.org/species/1689138</v>
       </c>
-      <c r="AA20" t="s">
+      <c r="AD20" t="s">
         <v>150</v>
       </c>
-      <c r="AB20" t="str">
-        <f t="shared" si="15"/>
+      <c r="AE20" t="str">
+        <f t="shared" si="16"/>
         <v>Hawaii</v>
       </c>
-      <c r="AC20" t="str">
-        <f t="shared" si="16"/>
+      <c r="AF20" t="str">
+        <f t="shared" si="17"/>
         <v>Kealakekua</v>
       </c>
-      <c r="AD20" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG20" t="str">
+        <f t="shared" si="18"/>
         <v>19°30′32′′N</v>
       </c>
-      <c r="AE20" t="str">
-        <f t="shared" si="18"/>
+      <c r="AH20" t="str">
+        <f t="shared" si="19"/>
         <v>155°51′46′′W</v>
       </c>
-      <c r="AF20">
-        <f t="shared" si="19"/>
+      <c r="AI20">
+        <f t="shared" si="20"/>
         <v>19.50888888888889</v>
       </c>
-      <c r="AG20">
-        <f t="shared" si="20"/>
+      <c r="AJ20">
+        <f t="shared" si="21"/>
         <v>-155.86277777777778</v>
       </c>
-      <c r="AH20" t="str">
-        <f t="shared" si="21"/>
+      <c r="AK20" t="str">
+        <f t="shared" si="22"/>
         <v>DQ649493|DQ649517</v>
       </c>
-      <c r="AI20" t="s">
+      <c r="AL20" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:35">
+    <row r="21" spans="1:38">
       <c r="A21" t="s">
         <v>113</v>
       </c>
@@ -3483,50 +3712,60 @@
       <c r="X21" t="s">
         <v>135</v>
       </c>
-      <c r="Y21" t="str">
+      <c r="Y21" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA21">
         <f t="shared" si="13"/>
+        <v>20</v>
+      </c>
+      <c r="AB21" t="str">
+        <f t="shared" si="14"/>
         <v>Banza nitida</v>
       </c>
-      <c r="Z21" t="str">
-        <f t="shared" si="14"/>
+      <c r="AC21" t="str">
+        <f t="shared" si="15"/>
         <v>http://www.gbif.org/species/1689138</v>
       </c>
-      <c r="AA21" t="s">
+      <c r="AD21" t="s">
         <v>150</v>
       </c>
-      <c r="AB21" t="str">
-        <f t="shared" si="15"/>
+      <c r="AE21" t="str">
+        <f t="shared" si="16"/>
         <v>Hawaii</v>
       </c>
-      <c r="AC21" t="str">
-        <f t="shared" si="16"/>
+      <c r="AF21" t="str">
+        <f t="shared" si="17"/>
         <v>Stainback</v>
       </c>
-      <c r="AD21" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG21" t="str">
+        <f t="shared" si="18"/>
         <v>19°34′14′′N</v>
       </c>
-      <c r="AE21" t="str">
-        <f t="shared" si="18"/>
+      <c r="AH21" t="str">
+        <f t="shared" si="19"/>
         <v>155°11′19′′W</v>
       </c>
-      <c r="AF21">
-        <f t="shared" si="19"/>
+      <c r="AI21">
+        <f t="shared" si="20"/>
         <v>19.570555555555554</v>
       </c>
-      <c r="AG21">
-        <f t="shared" si="20"/>
+      <c r="AJ21">
+        <f t="shared" si="21"/>
         <v>-155.18861111111113</v>
       </c>
-      <c r="AH21" t="str">
-        <f t="shared" si="21"/>
+      <c r="AK21" t="str">
+        <f t="shared" si="22"/>
         <v>DQ649495|DQ649519</v>
       </c>
-      <c r="AI21" t="s">
+      <c r="AL21" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:35">
+    <row r="22" spans="1:38">
       <c r="A22" t="s">
         <v>119</v>
       </c>
@@ -3609,46 +3848,56 @@
       <c r="X22" t="s">
         <v>135</v>
       </c>
-      <c r="Y22" t="str">
+      <c r="Y22" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA22">
         <f t="shared" si="13"/>
+        <v>21</v>
+      </c>
+      <c r="AB22" t="str">
+        <f t="shared" si="14"/>
         <v>Banza nitida</v>
       </c>
-      <c r="Z22" t="str">
-        <f t="shared" si="14"/>
+      <c r="AC22" t="str">
+        <f t="shared" si="15"/>
         <v>http://www.gbif.org/species/1689138</v>
       </c>
-      <c r="AA22" t="s">
+      <c r="AD22" t="s">
         <v>150</v>
       </c>
-      <c r="AB22" t="str">
-        <f t="shared" si="15"/>
+      <c r="AE22" t="str">
+        <f t="shared" si="16"/>
         <v>Hawaii</v>
       </c>
-      <c r="AC22" t="str">
-        <f t="shared" si="16"/>
+      <c r="AF22" t="str">
+        <f t="shared" si="17"/>
         <v>Puu Iki</v>
       </c>
-      <c r="AD22" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG22" t="str">
+        <f t="shared" si="18"/>
         <v>20°07′45′′N</v>
       </c>
-      <c r="AE22" t="str">
-        <f t="shared" si="18"/>
+      <c r="AH22" t="str">
+        <f t="shared" si="19"/>
         <v>155°46′09′′W</v>
       </c>
-      <c r="AF22">
-        <f t="shared" si="19"/>
+      <c r="AI22">
+        <f t="shared" si="20"/>
         <v>20.129166666666666</v>
       </c>
-      <c r="AG22">
-        <f t="shared" si="20"/>
+      <c r="AJ22">
+        <f t="shared" si="21"/>
         <v>-155.76916666666668</v>
       </c>
-      <c r="AH22" t="str">
-        <f t="shared" ref="AH22" si="22">CONCATENATE(F22,"|",G22)</f>
+      <c r="AK22" t="str">
+        <f t="shared" ref="AK22" si="23">CONCATENATE(F22,"|",G22)</f>
         <v>DQ649494|DQ649518</v>
       </c>
-      <c r="AI22" t="s">
+      <c r="AL22" t="s">
         <v>134</v>
       </c>
     </row>

</xml_diff>